<commit_message>
Añadida clase Config para cargar la ruta del archivo ventas.xlsx desde un txt
</commit_message>
<xml_diff>
--- a/ventas/ventas.xlsx
+++ b/ventas/ventas.xlsx
@@ -12,12 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Venta 0</t>
   </si>
   <si>
     <t>Venta 1</t>
+  </si>
+  <si>
+    <t>Venta 2</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -84,6 +87,14 @@
         <v>100.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>200.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
me when franco paez with mi balls
</commit_message>
<xml_diff>
--- a/ventas/ventas.xlsx
+++ b/ventas/ventas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Venta 0</t>
   </si>
@@ -21,6 +21,18 @@
   </si>
   <si>
     <t>Venta 2</t>
+  </si>
+  <si>
+    <t>Venta 3</t>
+  </si>
+  <si>
+    <t>Venta 4</t>
+  </si>
+  <si>
+    <t>Venta 5</t>
+  </si>
+  <si>
+    <t>Venta 6</t>
   </si>
 </sst>
 </file>
@@ -65,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -95,6 +107,38 @@
         <v>200.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>300.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>400.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>500.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>600.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Finalizada la funcionalidad para agregar ventas.
</commit_message>
<xml_diff>
--- a/ventas/ventas.xlsx
+++ b/ventas/ventas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>IdVentaTPS</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Monto</t>
   </si>
   <si>
-    <t>02/17/2025</t>
+    <t>02/44/2025</t>
   </si>
   <si>
     <t>Gaseosa 500ml</t>
@@ -56,7 +56,7 @@
     <t>Alfajor</t>
   </si>
   <si>
-    <t>02/18/2025</t>
+    <t>02/45/2025</t>
   </si>
 </sst>
 </file>
@@ -101,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -132,7 +132,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>750.0</v>
+        <v>2250.0</v>
       </c>
     </row>
     <row r="3">
@@ -160,7 +160,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>150.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="5">
@@ -174,7 +174,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>890.0</v>
+        <v>1780.0</v>
       </c>
     </row>
     <row r="6">
@@ -188,7 +188,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>240.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="7">
@@ -202,7 +202,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>1800.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="8">
@@ -230,7 +230,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>12500.0</v>
+        <v>10000.0</v>
       </c>
     </row>
     <row r="10">
@@ -244,133 +244,35 @@
         <v>13</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>1950.0</v>
+        <v>1300.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n" s="0">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>750.0</v>
+        <v>3560.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n" s="0">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>1560.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="D13" t="n" s="0">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D14" t="n" s="0">
-        <v>890.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D15" t="n" s="0">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D16" t="n" s="0">
-        <v>1200.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="D17" t="n" s="0">
-        <v>2100.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n" s="0">
-        <v>8.0</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D18" t="n" s="0">
-        <v>12500.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n" s="0">
-        <v>9.0</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D19" t="n" s="0">
-        <v>650.0</v>
+        <v>1300.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versión actualizada del ExcelWriter.
</commit_message>
<xml_diff>
--- a/ventas/ventas.xlsx
+++ b/ventas/ventas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>IdVentaTPS</t>
   </si>
@@ -23,10 +23,16 @@
     <t>Producto</t>
   </si>
   <si>
-    <t>Monto</t>
-  </si>
-  <si>
-    <t>02/44/2025</t>
+    <t>MontoBruto</t>
+  </si>
+  <si>
+    <t>MedioPago</t>
+  </si>
+  <si>
+    <t>DiagnósticoBot</t>
+  </si>
+  <si>
+    <t>02/12/2025</t>
   </si>
   <si>
     <t>Gaseosa 500ml</t>
@@ -54,9 +60,6 @@
   </si>
   <si>
     <t>Alfajor</t>
-  </si>
-  <si>
-    <t>02/45/2025</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -120,159 +123,137 @@
       <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>1.0</v>
+        <v>1.8293E7</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>2250.0</v>
+        <v>3750.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>2.0</v>
+        <v>1.8293001E7</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>1040.0</v>
+        <v>2080.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>3.0</v>
+        <v>1.8293002E7</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>100.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>4.0</v>
+        <v>1.8293003E7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>1780.0</v>
+        <v>890.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>5.0</v>
+        <v>1.8293004E7</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>80.0</v>
+        <v>320.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>6.0</v>
+        <v>1.8293005E7</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>1200.0</v>
+        <v>3000.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>7.0</v>
+        <v>1.8293006E7</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>2100.0</v>
+        <v>2800.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n" s="0">
-        <v>8.0</v>
+        <v>1.8293007E7</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>10000.0</v>
+        <v>12500.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n" s="0">
-        <v>9.0</v>
+        <v>1.8293008E7</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>1300.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D11" t="n" s="0">
-        <v>3560.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n" s="0">
-        <v>11.0</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D12" t="n" s="0">
-        <v>1300.0</v>
+        <v>650.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>